<commit_message>
Final commit with files clean up
</commit_message>
<xml_diff>
--- a/doc/sprint1/1191513/cable length.xlsx
+++ b/doc/sprint1/1191513/cable length.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JC\Dropbox\01 ISEP LEI\2 Ano\0202_RCOMP\Project\rcomp-20-21-dd-g5\doc\sprint1\1191513\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F05C98FD-0944-4A4D-B7E8-1D4488453CD1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9328071E-4029-46C3-B7D4-56AA0507246B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{D6EA5A22-4349-446F-9F1B-B6B838D7CC45}"/>
   </bookViews>
@@ -25,19 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
-  <si>
-    <t>Tomadas</t>
-  </si>
-  <si>
-    <t>B1G0</t>
-  </si>
-  <si>
-    <t>Sala 10.2 HC</t>
-  </si>
-  <si>
-    <t>sala 10.1 CP</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>desk</t>
   </si>
@@ -48,25 +36,37 @@
     <t>FIBRE</t>
   </si>
   <si>
-    <t>B1G1</t>
-  </si>
-  <si>
-    <t>CP</t>
-  </si>
-  <si>
-    <t>AP</t>
-  </si>
-  <si>
     <t>MC-HC</t>
   </si>
   <si>
-    <t>sala 11.2 HC</t>
-  </si>
-  <si>
-    <t>sala 11.3 CP</t>
-  </si>
-  <si>
-    <t>sala 11.4 CP</t>
+    <t>HC-&gt;CP</t>
+  </si>
+  <si>
+    <t>HC-&gt;AP</t>
+  </si>
+  <si>
+    <t>MC-&gt;HC</t>
+  </si>
+  <si>
+    <t>Sala 10.2 &lt;- HC</t>
+  </si>
+  <si>
+    <t>sala 10.1 &lt;- CP</t>
+  </si>
+  <si>
+    <t>sala 11.2 &lt;- HC</t>
+  </si>
+  <si>
+    <t>sala 11.3 &lt;- CP</t>
+  </si>
+  <si>
+    <t>sala 11.4 &lt;- CP</t>
+  </si>
+  <si>
+    <t>Building 1 Floor zero</t>
+  </si>
+  <si>
+    <t>Outlets</t>
   </si>
 </sst>
 </file>
@@ -82,15 +82,33 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC00FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -98,13 +116,140 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -113,6 +258,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCC00FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -421,522 +571,683 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C477047-3836-4FF8-AFDE-1BAB817FFBF7}">
-  <dimension ref="A1:I31"/>
+  <dimension ref="B2:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.109375" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="11.77734375" customWidth="1"/>
-    <col min="6" max="6" width="13.21875" customWidth="1"/>
-    <col min="7" max="7" width="13.77734375" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="7.5546875" customWidth="1"/>
+    <col min="6" max="6" width="11.77734375" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="H3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="9"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
+      <c r="C4" s="14"/>
+      <c r="D4" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="15"/>
+      <c r="F4" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="16"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B5" s="8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="8"/>
+      <c r="J5" s="9"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B6" s="1">
         <v>3</v>
       </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6">
+      <c r="C6" s="2">
         <f>3.5+2</f>
         <v>5.5</v>
       </c>
-      <c r="C6">
+      <c r="D6" s="5">
         <f>1.5+11.5+1.5+2</f>
         <v>16.5</v>
       </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6">
+      <c r="E6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1">
         <f>1+5.5+2+2</f>
         <v>10.5</v>
       </c>
-      <c r="F6">
+      <c r="G6" s="5">
         <v>4</v>
       </c>
-      <c r="G6">
+      <c r="H6" s="2">
         <f>1.5+2+2</f>
         <v>5.5</v>
       </c>
-      <c r="H6">
+      <c r="I6" s="1">
         <f>1+7+7.5+3</f>
         <v>18.5</v>
       </c>
-      <c r="I6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="J6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B7" s="1">
         <v>3</v>
       </c>
-      <c r="B7">
+      <c r="C7" s="2">
         <f>3.5+2</f>
         <v>5.5</v>
       </c>
-      <c r="C7">
+      <c r="D7" s="5">
         <f>1.5+8.5+8.5+4</f>
         <v>22.5</v>
       </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7">
+      <c r="E7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="1">
         <v>10.5</v>
       </c>
-      <c r="F7">
+      <c r="G7" s="5">
         <v>4</v>
       </c>
-      <c r="G7">
+      <c r="H7" s="2">
         <v>5.5</v>
       </c>
-      <c r="H7">
+      <c r="I7" s="1">
         <f>1+16+6.5+2</f>
         <v>25.5</v>
       </c>
-      <c r="I7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="J7" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B8" s="1">
         <v>8.5</v>
       </c>
-      <c r="B8">
+      <c r="C8" s="2">
         <f>3+2</f>
         <v>5</v>
       </c>
-      <c r="C8">
+      <c r="D8" s="5">
         <f>3.5+4+2.5</f>
         <v>10</v>
       </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8">
+      <c r="E8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="1">
         <f>8.5+3+2</f>
         <v>13.5</v>
       </c>
-      <c r="F8">
+      <c r="G8" s="5">
         <f>6+3+2</f>
         <v>11</v>
       </c>
-      <c r="G8">
+      <c r="H8" s="2">
         <f>1.5+5.5+2</f>
         <v>9</v>
       </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="I8" s="11">
+        <f>1+7+7.5+3</f>
+        <v>18.5</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B9" s="1">
         <v>8.5</v>
       </c>
-      <c r="B9">
+      <c r="C9" s="2">
         <v>5</v>
       </c>
-      <c r="E9">
+      <c r="D9" s="6">
+        <f>1.5+11.5+1.5+2</f>
+        <v>16.5</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="1">
         <v>13.5</v>
       </c>
-      <c r="F9">
+      <c r="G9" s="5">
         <v>11</v>
       </c>
-      <c r="G9">
+      <c r="H9" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="I9" s="11">
+        <f>1+16+6.5+2</f>
+        <v>25.5</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B10" s="1">
         <v>12</v>
       </c>
-      <c r="B10">
+      <c r="C10" s="2">
         <v>9</v>
       </c>
-      <c r="E10">
+      <c r="D10" s="6">
+        <f>1.5+8.5+8.5+4</f>
+        <v>22.5</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="1">
         <f>6.5+4.5+2+2</f>
         <v>15</v>
       </c>
-      <c r="F10">
+      <c r="G10" s="5">
         <v>5</v>
       </c>
-      <c r="G10">
+      <c r="H10" s="2">
         <f>1.5+9.5+2</f>
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B11" s="1">
         <v>12</v>
       </c>
-      <c r="B11">
+      <c r="C11" s="2">
         <v>9</v>
       </c>
-      <c r="E11">
+      <c r="D11" s="6">
+        <f>3.5+4+2.5</f>
+        <v>10</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="1">
         <v>15</v>
       </c>
-      <c r="F11">
+      <c r="G11" s="5">
         <v>5</v>
       </c>
-      <c r="G11">
+      <c r="H11" s="2">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="I11" s="1"/>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B12" s="1">
         <v>16</v>
       </c>
-      <c r="B12">
+      <c r="C12" s="2">
         <v>13</v>
       </c>
-      <c r="E12">
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="1">
         <f>6.5+1+2+2</f>
         <v>11.5</v>
       </c>
-      <c r="F12">
+      <c r="G12" s="5">
         <v>7.5</v>
       </c>
-      <c r="G12">
+      <c r="H12" s="2">
         <f>7+3.5+2</f>
         <v>12.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="I12" s="1"/>
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B13" s="1">
         <v>16</v>
       </c>
-      <c r="B13">
+      <c r="C13" s="2">
         <v>13</v>
       </c>
-      <c r="E13">
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="1">
         <v>11.5</v>
       </c>
-      <c r="F13">
+      <c r="G13" s="5">
         <v>7.5</v>
       </c>
-      <c r="G13">
+      <c r="H13" s="2">
         <v>12.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="I13" s="1"/>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B14" s="1">
         <f>11.5+6+2</f>
         <v>19.5</v>
       </c>
-      <c r="B14">
+      <c r="C14" s="2">
         <f>6.5+1.5+2</f>
         <v>10</v>
       </c>
-      <c r="E14">
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="1">
         <f>6.5+2.5+7.5+6</f>
         <v>22.5</v>
       </c>
-      <c r="F14">
+      <c r="G14" s="5">
         <v>11.5</v>
       </c>
-      <c r="G14">
+      <c r="H14" s="2">
         <f>7+7+2</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="I14" s="1"/>
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B15" s="1">
         <v>19.5</v>
       </c>
-      <c r="B15">
+      <c r="C15" s="2">
         <v>10</v>
       </c>
-      <c r="E15">
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="1">
         <v>22.5</v>
       </c>
-      <c r="F15">
+      <c r="G15" s="5">
         <v>11.5</v>
       </c>
-      <c r="G15">
+      <c r="H15" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="I15" s="1"/>
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B16" s="1">
         <f>11.5+9+2</f>
         <v>22.5</v>
       </c>
-      <c r="B16">
+      <c r="C16" s="2">
         <f>6.5+6+2</f>
         <v>14.5</v>
       </c>
-      <c r="F16">
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="5">
         <f>11.5+4+2</f>
         <v>17.5</v>
       </c>
-      <c r="G16">
+      <c r="H16" s="2">
         <f>1.5+11.5+2+2</f>
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="I16" s="1"/>
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B17" s="1">
         <v>22.5</v>
       </c>
-      <c r="B17">
+      <c r="C17" s="2">
         <v>14.5</v>
       </c>
-      <c r="F17">
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="5">
         <v>17.5</v>
       </c>
-      <c r="G17">
+      <c r="H17" s="2">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="I17" s="1"/>
+      <c r="J17" s="2"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B18" s="1">
         <f>11.5+11+1.5+2</f>
         <v>26</v>
       </c>
-      <c r="B18">
+      <c r="C18" s="2">
         <f>6.5+10+2</f>
         <v>18.5</v>
       </c>
-      <c r="F18">
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="5">
         <f>7+2+2</f>
         <v>11</v>
       </c>
-      <c r="G18">
+      <c r="H18" s="2">
         <f>13+5+2</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19">
+      <c r="I18" s="1"/>
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B19" s="1">
         <v>26</v>
       </c>
-      <c r="B19">
+      <c r="C19" s="2">
         <v>18.5</v>
       </c>
-      <c r="F19">
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="5">
         <v>11</v>
       </c>
-      <c r="G19">
+      <c r="H19" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20">
+      <c r="I19" s="1"/>
+      <c r="J19" s="2"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B20" s="1">
         <f>11.5+3.5+3.5+2</f>
         <v>20.5</v>
       </c>
-      <c r="B20">
+      <c r="C20" s="2">
         <f>6.5+11.5+3.5+2</f>
         <v>23.5</v>
       </c>
-      <c r="F20">
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="5">
         <f>7+5.5+2</f>
         <v>14.5</v>
       </c>
-      <c r="G20">
+      <c r="H20" s="2">
         <f>13+8+2</f>
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21">
+      <c r="I20" s="1"/>
+      <c r="J20" s="2"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B21" s="1">
         <v>20.5</v>
       </c>
-      <c r="B21">
+      <c r="C21" s="2">
         <v>23.5</v>
       </c>
-      <c r="F21">
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="5">
         <v>14.5</v>
       </c>
-      <c r="G21">
+      <c r="H21" s="2">
         <v>23</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22">
+      <c r="I21" s="1"/>
+      <c r="J21" s="2"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B22" s="1">
         <f>15+7.5+2</f>
         <v>24.5</v>
       </c>
-      <c r="B22">
+      <c r="C22" s="2">
         <f>6.5+11.5+7+1.5+2</f>
         <v>28.5</v>
       </c>
-      <c r="F22">
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="5">
         <f>7+9.5+2</f>
         <v>18.5</v>
       </c>
-      <c r="G22">
+      <c r="H22" s="2">
         <f>1.5+11+6.5+2</f>
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23">
+      <c r="I22" s="1"/>
+      <c r="J22" s="2"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B23" s="1">
         <v>24.5</v>
       </c>
-      <c r="B23">
+      <c r="C23" s="2">
         <v>28.5</v>
       </c>
-      <c r="F23">
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="5">
         <v>18.5</v>
       </c>
-      <c r="G23">
+      <c r="H23" s="2">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24">
+      <c r="I23" s="1"/>
+      <c r="J23" s="2"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B24" s="1">
         <f>11.5+7.5+3.5+2</f>
         <v>24.5</v>
       </c>
-      <c r="B24" t="s">
-        <v>4</v>
-      </c>
-      <c r="G24">
+      <c r="C24" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="2">
         <f>1.5+11+3+2</f>
         <v>17.5</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25">
+      <c r="I24" s="1"/>
+      <c r="J24" s="2"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B25" s="1">
         <v>24.5</v>
       </c>
-      <c r="B25">
+      <c r="C25" s="2">
         <f>1.5+1+3.5+27.5+3.5+0.5+2</f>
         <v>39.5</v>
       </c>
-      <c r="G25">
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="2">
         <v>17.5</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26">
+      <c r="I25" s="1"/>
+      <c r="J25" s="2"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B26" s="1">
         <f>11.5+7.5+7.5+2</f>
         <v>28.5</v>
       </c>
-      <c r="B26">
+      <c r="C26" s="2">
         <f>37.5+2</f>
         <v>39.5</v>
       </c>
-      <c r="G26">
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="2">
         <f>1.5+11+1.5+2</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27">
+      <c r="I26" s="1"/>
+      <c r="J26" s="2"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B27" s="1">
         <v>28.5</v>
       </c>
-      <c r="B27">
+      <c r="C27" s="2">
         <f>37+3.5+2</f>
         <v>42.5</v>
       </c>
-      <c r="G27">
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28">
+      <c r="I27" s="1"/>
+      <c r="J27" s="2"/>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B28" s="1">
         <f>1.5+11+1.5+2</f>
         <v>16</v>
       </c>
-      <c r="B28">
+      <c r="C28" s="2">
         <f>37+6.5+2</f>
         <v>45.5</v>
       </c>
-      <c r="G28">
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="2">
         <f>12.5+5.5+2</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29">
+      <c r="I28" s="1"/>
+      <c r="J28" s="2"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B29" s="1">
         <v>16</v>
       </c>
-      <c r="B29">
+      <c r="C29" s="2">
         <f>43.5+2</f>
         <v>45.5</v>
       </c>
-      <c r="G29">
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30">
+      <c r="I29" s="1"/>
+      <c r="J29" s="2"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B30" s="1">
         <f>1.5+11+1.5+2.5+2</f>
         <v>18.5</v>
       </c>
-      <c r="G30">
+      <c r="C30" s="2"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="2">
         <f>12.5+10+2</f>
         <v>24.5</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31">
+      <c r="I30" s="1"/>
+      <c r="J30" s="2"/>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B31" s="3">
         <v>18.5</v>
       </c>
-      <c r="G31">
+      <c r="C31" s="4"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="4">
         <v>24.5</v>
       </c>
+      <c r="I31" s="3"/>
+      <c r="J31" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="E3:F3"/>
+  <mergeCells count="4">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="I4:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>